<commit_message>
modified:   LandKreisKode.xlsx 	modified:   ParrallelScrap.py
</commit_message>
<xml_diff>
--- a/LandKreisKode.xlsx
+++ b/LandKreisKode.xlsx
@@ -873,8 +873,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="G38" sqref="G38"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="G71" sqref="G71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1667,7 +1667,7 @@
         <v>28</v>
       </c>
       <c r="G34">
-        <v>-2</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
@@ -1736,7 +1736,7 @@
         <v>28</v>
       </c>
       <c r="G37">
-        <v>-2</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
@@ -1782,7 +1782,7 @@
         <v>161</v>
       </c>
       <c r="G39">
-        <v>-1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
@@ -2127,7 +2127,7 @@
         <v>163</v>
       </c>
       <c r="G54">
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
@@ -2495,7 +2495,7 @@
         <v>165</v>
       </c>
       <c r="G70">
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
@@ -2541,7 +2541,7 @@
         <v>165</v>
       </c>
       <c r="G72">
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>